<commit_message>
Added Analytics Page Template
</commit_message>
<xml_diff>
--- a/_pipeline/input_temp_db/Rekap_BRCA12_Somatic_MAF_20210616_single.xlsx
+++ b/_pipeline/input_temp_db/Rekap_BRCA12_Somatic_MAF_20210616_single.xlsx
@@ -72,7 +72,7 @@
     <t>16/06/2021</t>
   </si>
   <si>
-    <t>dummy2_R2102170085</t>
+    <t>dummy_R2102170085X</t>
   </si>
   <si>
     <t>BRCA2</t>
@@ -1586,10 +1586,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1608,7 +1608,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1621,6 +1621,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1644,7 +1645,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1658,25 +1659,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1686,6 +1670,37 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1706,17 +1721,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1728,24 +1735,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1760,13 +1760,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1778,31 +1772,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1820,7 +1796,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1832,7 +1820,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1844,37 +1874,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1892,55 +1940,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1969,11 +1969,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2002,30 +2008,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2037,17 +2019,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2066,16 +2037,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2087,130 +2087,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2568,7 +2568,7 @@
   <dimension ref="A1:R201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>